<commit_message>
change the few requments
</commit_message>
<xml_diff>
--- a/downloads/Template.xlsx
+++ b/downloads/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\CELL_Block_Manager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\CELL_Block_Manager\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24E6413E-E409-4217-A8B3-46BCB062EC16}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9334BBC2-E978-4414-81A0-A975217FE7DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{7C1CD805-3218-4001-A288-BECE5999DFD8}"/>
+    <workbookView xWindow="348" yWindow="348" windowWidth="10728" windowHeight="6600" xr2:uid="{7C1CD805-3218-4001-A288-BECE5999DFD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <t>Site Name</t>
   </si>
   <si>
-    <t>BSC/RNC</t>
+    <t>Technology</t>
   </si>
 </sst>
 </file>
@@ -443,14 +443,14 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="57" customWidth="1"/>
   </cols>

</xml_diff>